<commit_message>
add weighted avg results for industry datasets
</commit_message>
<xml_diff>
--- a/Results/results_task4.xlsx
+++ b/Results/results_task4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeit\Papiere\NoRBERT\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005659D1-4C9E-447D-8D3A-58196DD3C617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E071796E-8C25-4C27-97B5-6F8385F9947C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EAA1F360-018B-4C01-84E1-44DDC1521104}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -162,7 +162,16 @@
     <t>OnlyF (54)</t>
   </si>
   <si>
-    <t>AVG:</t>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>weighted</t>
+  </si>
+  <si>
+    <t>Weighted AVG</t>
+  </si>
+  <si>
+    <t>Testset</t>
   </si>
 </sst>
 </file>
@@ -239,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,6 +271,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,13 +586,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABB2A89-5550-4106-AF63-C8C8FC55BBED}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2195,15 +2208,18 @@
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="4"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="4"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="5"/>
-      <c r="P33" s="7"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H34" s="2" t="s">
@@ -2470,172 +2486,175 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
+      <c r="G39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" ref="H39:I39" si="0">55*H36</f>
+        <v>55</v>
+      </c>
+      <c r="I39" s="5">
+        <f t="shared" si="0"/>
+        <v>46.75</v>
+      </c>
+      <c r="J39" s="5">
+        <f>55*J36</f>
+        <v>50.6</v>
+      </c>
+      <c r="K39" s="5">
+        <f>19*K36</f>
+        <v>7.7899999999999991</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" ref="L39" si="1">19*L38</f>
+        <v>16.91</v>
+      </c>
+      <c r="M39" s="5">
+        <f>19*M38</f>
+        <v>10.450000000000001</v>
+      </c>
+      <c r="N39" s="5">
+        <f>42*N36</f>
+        <v>42</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" ref="O39" si="2">42*O36</f>
+        <v>7.98</v>
+      </c>
+      <c r="P39" s="5">
+        <f>42*P37</f>
+        <v>27.720000000000002</v>
+      </c>
+      <c r="Q39" s="5">
+        <f>6*Q38</f>
+        <v>5.16</v>
+      </c>
+      <c r="R39" s="5">
+        <f t="shared" ref="R39:S39" si="3">6*R38</f>
+        <v>6</v>
+      </c>
+      <c r="S39" s="5">
+        <f t="shared" si="3"/>
+        <v>5.5200000000000005</v>
+      </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="7"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="2" t="s">
+      <c r="I42" s="3"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="2" t="s">
+      <c r="L42" s="3"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O41" s="3"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="1" t="s">
+      <c r="O42" s="3"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>6</v>
-      </c>
-      <c r="R42" t="s">
-        <v>7</v>
-      </c>
-      <c r="S42" t="s">
-        <v>8</v>
-      </c>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <v>16</v>
-      </c>
-      <c r="E43">
-        <v>42</v>
-      </c>
-      <c r="F43" t="b">
         <v>0</v>
       </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3</v>
+      </c>
       <c r="G43" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="I43" s="8">
-        <v>0.64</v>
-      </c>
-      <c r="J43" s="9">
-        <v>0.78</v>
-      </c>
-      <c r="K43" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="L43" s="8">
-        <v>0.95</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0.89</v>
-      </c>
-      <c r="N43" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="O43" s="8">
-        <v>0.65</v>
-      </c>
-      <c r="P43" s="9">
-        <v>0.64</v>
-      </c>
-      <c r="Q43">
-        <v>0.81</v>
-      </c>
-      <c r="R43" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="S43">
-        <v>0.87</v>
+        <v>4</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>6</v>
+      </c>
+      <c r="R43" t="s">
+        <v>7</v>
+      </c>
+      <c r="S43" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -2643,7 +2662,7 @@
         <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C44">
         <v>10</v>
@@ -2660,578 +2679,888 @@
       <c r="G44" t="s">
         <v>15</v>
       </c>
-      <c r="H44" s="12">
+      <c r="H44" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.78</v>
+      </c>
+      <c r="K44" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="M44" s="9">
+        <v>0.89</v>
+      </c>
+      <c r="N44" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="P44" s="9">
+        <v>0.64</v>
+      </c>
+      <c r="Q44">
+        <v>0.81</v>
+      </c>
+      <c r="R44" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="S44">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>16</v>
+      </c>
+      <c r="E45">
+        <v>42</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="12">
         <v>1</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I45" s="5">
         <v>0.61</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J45" s="7">
         <v>0.76</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K45" s="4">
         <v>0.8</v>
       </c>
-      <c r="L44" s="5">
+      <c r="L45" s="5">
         <v>0.9</v>
       </c>
-      <c r="M44" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="N44" s="12">
+      <c r="M45" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="N45" s="12">
         <v>0.67</v>
       </c>
-      <c r="O44" s="5">
+      <c r="O45" s="5">
         <v>0.52</v>
       </c>
-      <c r="P44" s="7">
+      <c r="P45" s="7">
         <v>0.59</v>
       </c>
-      <c r="Q44" s="10">
+      <c r="Q45" s="10">
         <v>0.9</v>
       </c>
-      <c r="R44" s="10">
+      <c r="R45" s="10">
         <v>0.95</v>
       </c>
-      <c r="S44" s="10">
+      <c r="S45" s="10">
         <v>0.93</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-    </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="7"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H46" s="5">
+        <f>44*H45</f>
+        <v>44</v>
+      </c>
+      <c r="I46" s="5">
+        <f t="shared" ref="I46" si="4">44*I44</f>
+        <v>28.16</v>
+      </c>
+      <c r="J46" s="5">
+        <f>44*J44</f>
+        <v>34.32</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" ref="K46:L46" si="5">61*K44</f>
+        <v>51.239999999999995</v>
+      </c>
+      <c r="L46" s="5">
+        <f t="shared" si="5"/>
+        <v>57.949999999999996</v>
+      </c>
+      <c r="M46" s="5">
+        <f>61*M44</f>
+        <v>54.29</v>
+      </c>
+      <c r="N46" s="5">
+        <f>23*N45</f>
+        <v>15.41</v>
+      </c>
+      <c r="O46" s="5">
+        <f t="shared" ref="O46:P46" si="6">23*O44</f>
+        <v>14.950000000000001</v>
+      </c>
+      <c r="P46" s="5">
+        <f t="shared" si="6"/>
+        <v>14.72</v>
+      </c>
+      <c r="Q46" s="5">
+        <f>40*Q45</f>
+        <v>36</v>
+      </c>
+      <c r="R46" s="5">
+        <f t="shared" ref="R46:S46" si="7">40*R45</f>
+        <v>38</v>
+      </c>
+      <c r="S46" s="5">
+        <f t="shared" si="7"/>
+        <v>37.200000000000003</v>
+      </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H47" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O47" s="3"/>
-      <c r="P47" s="6"/>
-      <c r="Q47" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H49" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49" s="3"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O49" s="3"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>0</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D50" t="s">
         <v>13</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E50" t="s">
         <v>2</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
         <v>3</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G50" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="7" t="s">
+      <c r="J50" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="L50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M48" s="7" t="s">
+      <c r="M50" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N48" s="4" t="s">
+      <c r="N50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O48" s="5" t="s">
+      <c r="O50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P48" s="7" t="s">
+      <c r="P50" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="Q50" t="s">
         <v>6</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R50" t="s">
         <v>7</v>
       </c>
-      <c r="S48" t="s">
+      <c r="S50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>34</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>14</v>
       </c>
-      <c r="C49">
+      <c r="C51">
         <v>10</v>
       </c>
-      <c r="D49">
-        <v>16</v>
-      </c>
-      <c r="E49">
+      <c r="D51">
+        <v>16</v>
+      </c>
+      <c r="E51">
         <v>42</v>
       </c>
-      <c r="F49" t="b">
+      <c r="F51" t="b">
         <v>0</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G51" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H51" s="4">
         <v>0.97</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I51" s="8">
         <v>0.97</v>
       </c>
-      <c r="J49" s="7">
+      <c r="J51" s="7">
         <v>0.98</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K51" s="4">
         <v>0.71</v>
       </c>
-      <c r="L49" s="5">
+      <c r="L51" s="5">
         <v>0.47</v>
       </c>
-      <c r="M49" s="7">
+      <c r="M51" s="7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N49" s="12">
+      <c r="N51" s="12">
         <v>0.84</v>
       </c>
-      <c r="O49" s="5">
+      <c r="O51" s="5">
         <v>0.48</v>
       </c>
-      <c r="P49" s="7">
+      <c r="P51" s="7">
         <v>0.61</v>
       </c>
-      <c r="Q49">
+      <c r="Q51">
         <v>0.6</v>
       </c>
-      <c r="R49">
+      <c r="R51">
         <v>0.82</v>
       </c>
-      <c r="S49">
+      <c r="S51">
         <v>0.69</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>34</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>18</v>
       </c>
-      <c r="C50">
+      <c r="C52">
         <v>10</v>
       </c>
-      <c r="D50">
-        <v>16</v>
-      </c>
-      <c r="E50">
+      <c r="D52">
+        <v>16</v>
+      </c>
+      <c r="E52">
         <v>42</v>
       </c>
-      <c r="F50" t="b">
+      <c r="F52" t="b">
         <v>0</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G52" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="12">
+      <c r="H52" s="12">
         <v>1</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I52" s="8">
         <v>0.97</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J52" s="9">
         <v>0.99</v>
       </c>
-      <c r="K50" s="12">
+      <c r="K52" s="12">
         <v>0.73</v>
       </c>
-      <c r="L50" s="8">
+      <c r="L52" s="8">
         <v>0.59</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M52" s="9">
         <v>0.66</v>
       </c>
-      <c r="N50" s="4">
+      <c r="N52" s="4">
         <v>0.82</v>
       </c>
-      <c r="O50" s="8">
+      <c r="O52" s="8">
         <v>0.67</v>
       </c>
-      <c r="P50" s="9">
+      <c r="P52" s="9">
         <v>0.73</v>
       </c>
-      <c r="Q50" s="11">
+      <c r="Q52" s="11">
         <v>0.83</v>
       </c>
-      <c r="R50" s="11">
+      <c r="R52" s="11">
         <v>0.91</v>
       </c>
-      <c r="S50" s="11">
+      <c r="S52" s="11">
         <v>0.87</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" ref="H53:I53" si="8">75*H52</f>
+        <v>75</v>
+      </c>
+      <c r="I53" s="5">
+        <f t="shared" si="8"/>
+        <v>72.75</v>
+      </c>
+      <c r="J53" s="5">
+        <f>75*J52</f>
+        <v>74.25</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" ref="K53:L53" si="9">32*K52</f>
+        <v>23.36</v>
+      </c>
+      <c r="L53" s="5">
+        <f t="shared" si="9"/>
+        <v>18.88</v>
+      </c>
+      <c r="M53" s="5">
+        <f>32*M52</f>
+        <v>21.12</v>
+      </c>
+      <c r="N53" s="5">
+        <f>54*N51</f>
+        <v>45.36</v>
+      </c>
+      <c r="O53" s="5">
+        <f t="shared" ref="O53:P53" si="10">54*O52</f>
+        <v>36.18</v>
+      </c>
+      <c r="P53" s="5">
+        <f t="shared" si="10"/>
+        <v>39.42</v>
+      </c>
+      <c r="Q53" s="5">
+        <f>11*Q52</f>
+        <v>9.129999999999999</v>
+      </c>
+      <c r="R53" s="5">
+        <f t="shared" ref="R53:S53" si="11">11*R52</f>
+        <v>10.01</v>
+      </c>
+      <c r="S53" s="5">
+        <f t="shared" si="11"/>
+        <v>9.57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="7"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H53" s="2" t="s">
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H56" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="2" t="s">
+      <c r="I56" s="3"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L53" s="3"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="2" t="s">
+      <c r="L56" s="3"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O53" s="3"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="1" t="s">
+      <c r="O56" s="3"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>0</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C57" t="s">
         <v>1</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>13</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E57" t="s">
         <v>2</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F57" t="s">
         <v>3</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G57" t="s">
         <v>4</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="I57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J54" s="7" t="s">
+      <c r="J57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K54" s="4" t="s">
+      <c r="K57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="L57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M54" s="7" t="s">
+      <c r="M57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N54" s="4" t="s">
+      <c r="N57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="O54" s="5" t="s">
+      <c r="O57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P54" s="7" t="s">
+      <c r="P57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="Q57" t="s">
         <v>6</v>
       </c>
-      <c r="R54" t="s">
+      <c r="R57" t="s">
         <v>7</v>
       </c>
-      <c r="S54" t="s">
+      <c r="S57" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>34</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>14</v>
       </c>
-      <c r="C55">
+      <c r="C58">
         <v>10</v>
       </c>
-      <c r="D55">
-        <v>16</v>
-      </c>
-      <c r="E55">
+      <c r="D58">
+        <v>16</v>
+      </c>
+      <c r="E58">
         <v>42</v>
       </c>
-      <c r="F55" t="b">
+      <c r="F58" t="b">
         <v>0</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G58" t="s">
         <v>15</v>
       </c>
-      <c r="H55" s="12">
+      <c r="H58" s="12">
         <v>0.98</v>
       </c>
-      <c r="I55" s="5">
+      <c r="I58" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J55" s="7">
+      <c r="J58" s="7">
         <v>0.71</v>
       </c>
-      <c r="K55" s="4">
+      <c r="K58" s="4">
         <v>0.6</v>
       </c>
-      <c r="L55" s="5">
+      <c r="L58" s="5">
         <v>0.43</v>
       </c>
-      <c r="M55" s="7">
+      <c r="M58" s="7">
         <v>0.5</v>
       </c>
-      <c r="N55" s="12">
+      <c r="N58" s="12">
         <v>0.93</v>
       </c>
-      <c r="O55" s="5">
+      <c r="O58" s="5">
         <v>0.38</v>
       </c>
-      <c r="P55" s="7">
+      <c r="P58" s="7">
         <v>0.54</v>
       </c>
-      <c r="Q55">
+      <c r="Q58">
         <v>0</v>
       </c>
-      <c r="R55">
+      <c r="R58">
         <v>0</v>
       </c>
-      <c r="S55">
+      <c r="S58">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>34</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>18</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>10</v>
       </c>
-      <c r="D56">
-        <v>16</v>
-      </c>
-      <c r="E56">
+      <c r="D59">
+        <v>16</v>
+      </c>
+      <c r="E59">
         <v>42</v>
       </c>
-      <c r="F56" t="b">
+      <c r="F59" t="b">
         <v>0</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G59" t="s">
         <v>15</v>
       </c>
-      <c r="H56" s="12">
+      <c r="H59" s="12">
         <v>0.98</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I59" s="8">
         <v>0.84</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J59" s="9">
         <v>0.9</v>
       </c>
-      <c r="K56" s="12">
+      <c r="K59" s="12">
         <v>0.62</v>
       </c>
-      <c r="L56" s="8">
+      <c r="L59" s="8">
         <v>0.46</v>
       </c>
-      <c r="M56" s="9">
+      <c r="M59" s="9">
         <v>0.53</v>
       </c>
-      <c r="N56" s="4">
+      <c r="N59" s="4">
         <v>0.81</v>
       </c>
-      <c r="O56" s="8">
+      <c r="O59" s="8">
         <v>0.63</v>
       </c>
-      <c r="P56" s="9">
+      <c r="P59" s="9">
         <v>0.71</v>
       </c>
-      <c r="Q56" s="11">
+      <c r="Q59" s="11">
         <v>0.08</v>
       </c>
-      <c r="R56" s="11">
+      <c r="R59" s="11">
         <v>0.5</v>
       </c>
-      <c r="S56" s="11">
+      <c r="S59" s="11">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G58" t="s">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G60" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60">
+        <f t="shared" ref="H60:I60" si="12">94*H59</f>
+        <v>92.12</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="12"/>
+        <v>78.959999999999994</v>
+      </c>
+      <c r="J60">
+        <f>94*J59</f>
+        <v>84.600000000000009</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:L60" si="13">28*K59</f>
+        <v>17.36</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="13"/>
+        <v>12.88</v>
+      </c>
+      <c r="M60">
+        <f>28*M59</f>
+        <v>14.84</v>
+      </c>
+      <c r="N60">
+        <f>68*N58</f>
+        <v>63.24</v>
+      </c>
+      <c r="O60">
+        <f t="shared" ref="O60:P60" si="14">68*O59</f>
+        <v>42.84</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="14"/>
+        <v>48.28</v>
+      </c>
+      <c r="Q60">
+        <f>2*Q59</f>
+        <v>0.16</v>
+      </c>
+      <c r="R60">
+        <f t="shared" ref="R60:S60" si="15">2*R59</f>
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="15"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <f>55+44+75+94</f>
+        <v>268</v>
+      </c>
+      <c r="L62">
+        <f>28+32+61+19</f>
+        <v>140</v>
+      </c>
+      <c r="O62">
+        <f>42+23+54+68</f>
+        <v>187</v>
+      </c>
+      <c r="R62">
+        <f>2+11+40+6</f>
+        <v>59</v>
+      </c>
+      <c r="T62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H63" s="14">
+        <f t="shared" ref="H63:I63" si="16">SUM(H39,H46,H53,H60)/(55+44+75+94)</f>
+        <v>0.99298507462686569</v>
+      </c>
+      <c r="I63" s="14">
+        <f t="shared" si="16"/>
+        <v>0.8455970149253732</v>
+      </c>
+      <c r="J63" s="14">
+        <f>SUM(J39,J46,J53,J60)/(55+44+75+94)</f>
+        <v>0.90958955223880611</v>
+      </c>
+      <c r="K63" s="14">
+        <f>SUM(K39,K46,K53,K60)/(19+61+32+28)</f>
+        <v>0.71249999999999991</v>
+      </c>
+      <c r="L63" s="14">
+        <f t="shared" ref="L63:M63" si="17">SUM(L39,L46,L53,L60)/(19+61+32+28)</f>
+        <v>0.76157142857142845</v>
+      </c>
+      <c r="M63" s="14">
+        <f t="shared" si="17"/>
+        <v>0.71928571428571431</v>
+      </c>
+      <c r="N63" s="14">
+        <f>SUM(N39,N46,N53,N60)/(42+23+54+68)</f>
+        <v>0.88775401069518711</v>
+      </c>
+      <c r="O63" s="14">
+        <f t="shared" ref="O63:P63" si="18">SUM(O39,O46,O53,O60)/(42+23+54+68)</f>
+        <v>0.54518716577540105</v>
+      </c>
+      <c r="P63" s="14">
+        <f t="shared" si="18"/>
+        <v>0.69593582887700545</v>
+      </c>
+      <c r="Q63" s="14">
+        <f>SUM(Q39,Q46,Q53,Q60)/(6+40+11+2)</f>
+        <v>0.85508474576271165</v>
+      </c>
+      <c r="R63" s="14">
+        <f t="shared" ref="R63:S63" si="19">SUM(R39,R46,R53,R60)/(6+40+11+2)</f>
+        <v>0.93237288135593221</v>
+      </c>
+      <c r="S63" s="14">
+        <f t="shared" si="19"/>
+        <v>0.89101694915254248</v>
+      </c>
+      <c r="T63" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H64" s="14">
+        <f>AVERAGE(H38,H45,H52,H59)</f>
+        <v>0.995</v>
+      </c>
+      <c r="I64" s="14">
+        <f>AVERAGE(I36,I44,I52,I59)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="J64" s="14">
+        <f>AVERAGE(J36,J44,J52,J59)</f>
+        <v>0.89750000000000008</v>
+      </c>
+      <c r="K64" s="14">
+        <f>AVERAGE(K36,K44,K52,K59)</f>
+        <v>0.65</v>
+      </c>
+      <c r="L64" s="14">
+        <f>AVERAGE(L38,L44,L52,L59)</f>
+        <v>0.72249999999999992</v>
+      </c>
+      <c r="M64" s="14">
+        <f>AVERAGE(M38,M44,M52,M59)</f>
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="N64" s="14">
+        <f>AVERAGE(N36,N45,N51,N58)</f>
+        <v>0.86</v>
+      </c>
+      <c r="O64" s="14">
+        <f>AVERAGE(O36,O44,O52,O59)</f>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="P64" s="14">
+        <f>AVERAGE(P37,P44,P52,P59)</f>
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="Q64" s="14">
+        <f>AVERAGE(Q38,Q45,Q52,Q59)</f>
+        <v>0.66749999999999998</v>
+      </c>
+      <c r="R64" s="14">
+        <f>AVERAGE(R38,R45,R52,R59)</f>
+        <v>0.84</v>
+      </c>
+      <c r="S64" s="14">
+        <f>AVERAGE(S38,S45,S52,S59)</f>
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="T64" t="s">
         <v>45</v>
-      </c>
-      <c r="H58">
-        <f>AVERAGE(H36:H38,H43,H44,H49,H50,H55,H56)</f>
-        <v>0.98888888888888893</v>
-      </c>
-      <c r="I58">
-        <f>AVERAGE(I36:I38,I43,I44,I49,I50,I55,I56)</f>
-        <v>0.75777777777777766</v>
-      </c>
-      <c r="J58">
-        <f>AVERAGE(J36:J38,J43,J44,J49,J50,J55,J56)</f>
-        <v>0.85222222222222233</v>
-      </c>
-      <c r="K58">
-        <f>AVERAGE(K36:K38,K43,K44,K49,K50,K55,K56)</f>
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="L58">
-        <f>AVERAGE(L36:L38,L43,L44,L49,L50,L55,L56)</f>
-        <v>0.70222222222222219</v>
-      </c>
-      <c r="M58">
-        <f>AVERAGE(M36:M38,M43,M44,M49,M50,M55,M56)</f>
-        <v>0.62555555555555553</v>
-      </c>
-      <c r="N58">
-        <f>AVERAGE(N36:N38,N43,N44,N49,N50,N55,N56)</f>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="O58">
-        <f>AVERAGE(O36:O38,O43,O44,O49,O50,O55,O56)</f>
-        <v>0.46555555555555561</v>
-      </c>
-      <c r="P58">
-        <f>AVERAGE(P36:P38,P43,P44,P49,P50,P55,P56)</f>
-        <v>0.56555555555555559</v>
-      </c>
-      <c r="Q58">
-        <f>AVERAGE(Q36:Q38,Q43,Q44,Q49,Q50,Q55,Q56)</f>
-        <v>0.55222222222222217</v>
-      </c>
-      <c r="R58">
-        <f>AVERAGE(R36:R38,R43,R44,R49,R50,R55,R56)</f>
-        <v>0.79222222222222227</v>
-      </c>
-      <c r="S58">
-        <f>AVERAGE(S36:S38,S43,S44,S49,S50,S55,S56)</f>
-        <v>0.62333333333333329</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="Q41:S41"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="Q49:S49"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>

</xml_diff>